<commit_message>
created personal sites for every profile
</commit_message>
<xml_diff>
--- a/public/Heropoints.xlsx
+++ b/public/Heropoints.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Anti-Mage</t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t>Hoodwink</t>
+  </si>
+  <si>
+    <t>Grimstroke</t>
+  </si>
+  <si>
+    <t>Mars</t>
   </si>
 </sst>
 </file>
@@ -386,12 +392,12 @@
       <color rgb="FF032F62"/>
       <name val="SFMono-Regular"/>
     </font>
+    <font/>
     <font>
       <sz val="9.0"/>
       <color rgb="FF032F62"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -423,10 +429,10 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -652,8 +658,8 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
-        <v>0.0</v>
+      <c r="C1" s="3">
+        <v>-8.0</v>
       </c>
       <c r="D1" s="2"/>
     </row>
@@ -664,8 +670,8 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.0</v>
+      <c r="C2" s="3">
+        <v>-2.0</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -685,13 +691,13 @@
       <c r="A4" s="1">
         <v>4.0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>5.0</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1">
@@ -733,7 +739,7 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>8.0</v>
       </c>
     </row>
@@ -755,8 +761,8 @@
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.0</v>
+      <c r="C10" s="3">
+        <v>-15.0</v>
       </c>
     </row>
     <row r="11">
@@ -766,8 +772,8 @@
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.0</v>
+      <c r="C11" s="3">
+        <v>-2.0</v>
       </c>
     </row>
     <row r="12">
@@ -876,7 +882,7 @@
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>5.0</v>
       </c>
     </row>
@@ -994,7 +1000,7 @@
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>-10.0</v>
       </c>
     </row>
@@ -1038,7 +1044,7 @@
       <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>15.0</v>
       </c>
     </row>
@@ -1126,7 +1132,7 @@
       <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>3.0</v>
       </c>
     </row>
@@ -1225,7 +1231,7 @@
       <c r="B53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="3">
         <v>-20.0</v>
       </c>
     </row>
@@ -1486,7 +1492,7 @@
       <c r="A77" s="1">
         <v>77.0</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C77" s="1">
@@ -1588,8 +1594,8 @@
       <c r="B86" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="1">
-        <v>0.0</v>
+      <c r="C86" s="3">
+        <v>4.0</v>
       </c>
     </row>
     <row r="87">
@@ -1643,7 +1649,7 @@
       <c r="B91" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91" s="3">
         <v>-10.0</v>
       </c>
     </row>
@@ -1676,7 +1682,7 @@
       <c r="B94" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94" s="3">
         <v>-5.0</v>
       </c>
     </row>
@@ -1783,7 +1789,7 @@
       <c r="A104" s="1">
         <v>104.0</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C104" s="1">
@@ -1797,7 +1803,7 @@
       <c r="B105" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C105" s="3">
         <v>-100.0</v>
       </c>
     </row>
@@ -1830,7 +1836,7 @@
       <c r="B108" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C108" s="3">
         <v>15.0</v>
       </c>
     </row>
@@ -1885,7 +1891,7 @@
       <c r="B113" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C113" s="4">
+      <c r="C113" s="3">
         <v>-50.0</v>
       </c>
     </row>
@@ -1918,7 +1924,7 @@
       <c r="B116" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="4">
+      <c r="C116" s="3">
         <v>10.0</v>
       </c>
     </row>
@@ -1948,11 +1954,33 @@
       <c r="A119" s="1">
         <v>123.0</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C119" s="1">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1">
+        <v>121.0</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C120" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1">
+        <v>129.0</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121" s="1">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>